<commit_message>
format and feat detail
</commit_message>
<xml_diff>
--- a/aikataulutus/Tyotunnit.xlsx
+++ b/aikataulutus/Tyotunnit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riku\Koulu\Ohjelmointyo\aikataulutus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50D4E07-7DE3-45C4-A506-9E0635D0A5E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DDFC1C5-E77F-4979-9D86-4121335B5927}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="195" windowWidth="21600" windowHeight="11400" xr2:uid="{645D6CBF-11AA-407D-8E7D-16FD02D07F5D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{645D6CBF-11AA-407D-8E7D-16FD02D07F5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Paivamaara</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>tietokannan maarittelya</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -422,7 +425,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,8 +486,21 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D4" s="3"/>
-      <c r="E4" s="4"/>
+      <c r="A4" s="1">
+        <v>44047</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D5" s="3"/>

</xml_diff>

<commit_message>
ancestry ja tunnit formatointi
</commit_message>
<xml_diff>
--- a/aikataulutus/Tyotunnit.xlsx
+++ b/aikataulutus/Tyotunnit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riku\Koulu\Ohjelmointyo\aikataulutus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE62C27-8D91-4095-8C9E-47541472A145}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4963DBB-35F6-48D7-8249-318F48FB3DC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="585" windowWidth="21600" windowHeight="11400" xr2:uid="{645D6CBF-11AA-407D-8E7D-16FD02D07F5D}"/>
+    <workbookView xWindow="3885" yWindow="1380" windowWidth="21600" windowHeight="11400" xr2:uid="{645D6CBF-11AA-407D-8E7D-16FD02D07F5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Paivamaara</t>
   </si>
@@ -63,15 +63,15 @@
   </si>
   <si>
     <t>Total Tunnit</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -101,7 +101,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -115,6 +115,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
@@ -472,15 +477,16 @@
       <c r="C2" s="2">
         <v>0.73958333333333337</v>
       </c>
-      <c r="D2" s="5">
-        <v>1.25</v>
+      <c r="D2" s="8">
+        <f>C2-B2</f>
+        <v>5.208333333333337E-2</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="9">
         <f>D2</f>
-        <v>1.25</v>
+        <v>5.208333333333337E-2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -493,15 +499,16 @@
       <c r="C3" s="2">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D3" s="3">
-        <v>3</v>
+      <c r="D3" s="8">
+        <f t="shared" ref="D3:D13" si="0">C3-B3</f>
+        <v>0.125</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="9">
         <f>F2+D3</f>
-        <v>4.25</v>
+        <v>0.17708333333333337</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -514,15 +521,16 @@
       <c r="C4" s="2">
         <v>0.77083333333333337</v>
       </c>
-      <c r="D4" s="3">
-        <v>3</v>
+      <c r="D4" s="8">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="9">
         <f>F3+D4</f>
-        <v>7.25</v>
+        <v>0.30208333333333337</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -535,15 +543,16 @@
       <c r="C5" s="2">
         <v>0.94791666666666663</v>
       </c>
-      <c r="D5" s="3">
-        <v>5.75</v>
+      <c r="D5" s="8">
+        <f t="shared" si="0"/>
+        <v>0.23958333333333326</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="6">
-        <f t="shared" ref="F5:F6" si="0">F4+D5</f>
-        <v>13</v>
+      <c r="F5" s="9">
+        <f t="shared" ref="F5:F13" si="1">F4+D5</f>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -556,15 +565,16 @@
       <c r="C6" s="2">
         <v>0.78125</v>
       </c>
-      <c r="D6" s="3">
-        <v>4</v>
+      <c r="D6" s="8">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666663</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="6">
-        <f t="shared" si="0"/>
-        <v>17</v>
+      <c r="F6" s="9">
+        <f t="shared" si="1"/>
+        <v>0.70833333333333326</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -574,45 +584,95 @@
       <c r="B7" s="2">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="4"/>
+      <c r="C7" s="2">
+        <v>7.9861111111111105E-2</v>
+      </c>
+      <c r="D7" s="8">
+        <f t="shared" si="0"/>
+        <v>6.9444444444444434E-2</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="9">
+        <f t="shared" si="1"/>
+        <v>0.77777777777777768</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D8" s="5"/>
+      <c r="D8" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E8" s="4"/>
+      <c r="F8" s="9">
+        <f t="shared" si="1"/>
+        <v>0.77777777777777768</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D9" s="5"/>
+      <c r="D9" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E9" s="4"/>
+      <c r="F9" s="9">
+        <f t="shared" si="1"/>
+        <v>0.77777777777777768</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D10" s="5"/>
+      <c r="B10" s="7"/>
+      <c r="D10" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E10" s="4"/>
+      <c r="F10" s="9">
+        <f t="shared" si="1"/>
+        <v>0.77777777777777768</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D11" s="5"/>
+      <c r="D11" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E11" s="4"/>
+      <c r="F11" s="9">
+        <f t="shared" si="1"/>
+        <v>0.77777777777777768</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D12" s="5"/>
-      <c r="E12" s="4"/>
+      <c r="D12" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="9">
+        <f t="shared" si="1"/>
+        <v>0.77777777777777768</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D13" s="5"/>
-      <c r="E13" s="4"/>
+      <c r="D13" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="9">
+        <f t="shared" si="1"/>
+        <v>0.77777777777777768</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D14" s="5"/>
-      <c r="E14" s="4"/>
+      <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D15" s="5"/>
-      <c r="E15" s="4"/>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D16" s="5"/>

</xml_diff>

<commit_message>
6.9 - XML ja database korjaus ja maarittely
</commit_message>
<xml_diff>
--- a/aikataulutus/Tyotunnit.xlsx
+++ b/aikataulutus/Tyotunnit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riku\Koulu\Ohjelmointyo\aikataulutus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29450D34-EF93-4274-9263-8AC50C8C4968}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19FDCB2-31B5-4AA5-8005-0AD25E1BE835}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{645D6CBF-11AA-407D-8E7D-16FD02D07F5D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Paivamaara</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>xml + unity</t>
+  </si>
+  <si>
+    <t>xml toimii unityssa</t>
+  </si>
+  <si>
+    <t>database uudelleenmaarittely + unity</t>
   </si>
 </sst>
 </file>
@@ -448,7 +454,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,22 +723,35 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>44079</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C13" s="9">
+        <v>1.03125</v>
+      </c>
       <c r="D13" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E13" s="3"/>
+        <v>0.19791666666666663</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="F13" s="10">
         <f t="shared" si="1"/>
-        <v>1.2361111111111109</v>
+        <v>1.4340277777777777</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D14" s="5"/>
-      <c r="E14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="F14" s="10">
         <f t="shared" si="1"/>
-        <v>1.2361111111111109</v>
+        <v>1.4340277777777777</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -740,7 +759,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="10">
         <f t="shared" si="1"/>
-        <v>1.2361111111111109</v>
+        <v>1.4340277777777777</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -748,7 +767,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="10">
         <f t="shared" si="1"/>
-        <v>1.2361111111111109</v>
+        <v>1.4340277777777777</v>
       </c>
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.25">
@@ -756,7 +775,7 @@
       <c r="E17" s="4"/>
       <c r="F17" s="10">
         <f t="shared" si="1"/>
-        <v>1.2361111111111109</v>
+        <v>1.4340277777777777</v>
       </c>
     </row>
     <row r="18" spans="4:6" x14ac:dyDescent="0.25">
@@ -764,7 +783,7 @@
       <c r="E18" s="4"/>
       <c r="F18" s="10">
         <f t="shared" si="1"/>
-        <v>1.2361111111111109</v>
+        <v>1.4340277777777777</v>
       </c>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.25">
@@ -772,7 +791,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="10">
         <f t="shared" si="1"/>
-        <v>1.2361111111111109</v>
+        <v>1.4340277777777777</v>
       </c>
     </row>
     <row r="20" spans="4:6" x14ac:dyDescent="0.25">
@@ -780,7 +799,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="10">
         <f t="shared" si="1"/>
-        <v>1.2361111111111109</v>
+        <v>1.4340277777777777</v>
       </c>
     </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.25">
@@ -788,40 +807,40 @@
       <c r="E21" s="4"/>
       <c r="F21" s="10">
         <f t="shared" si="1"/>
-        <v>1.2361111111111109</v>
+        <v>1.4340277777777777</v>
       </c>
     </row>
     <row r="22" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D22" s="5"/>
       <c r="F22" s="10">
         <f t="shared" si="1"/>
-        <v>1.2361111111111109</v>
+        <v>1.4340277777777777</v>
       </c>
     </row>
     <row r="23" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D23" s="5"/>
       <c r="F23" s="10">
         <f t="shared" si="1"/>
-        <v>1.2361111111111109</v>
+        <v>1.4340277777777777</v>
       </c>
     </row>
     <row r="24" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D24" s="6"/>
       <c r="F24" s="10">
         <f t="shared" si="1"/>
-        <v>1.2361111111111109</v>
+        <v>1.4340277777777777</v>
       </c>
     </row>
     <row r="25" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F25" s="10">
         <f t="shared" si="1"/>
-        <v>1.2361111111111109</v>
+        <v>1.4340277777777777</v>
       </c>
     </row>
     <row r="26" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F26" s="10">
         <f t="shared" si="1"/>
-        <v>1.2361111111111109</v>
+        <v>1.4340277777777777</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UI + XML + Character info
</commit_message>
<xml_diff>
--- a/aikataulutus/Tyotunnit.xlsx
+++ b/aikataulutus/Tyotunnit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riku\Koulu\Ohjelmointyo\aikataulutus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69CDBC5D-05C4-4E90-B745-85FFDF261B13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94FF0D0-6C31-4689-8A24-5A6A2CC639DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32175" yWindow="1815" windowWidth="19665" windowHeight="12780" xr2:uid="{645D6CBF-11AA-407D-8E7D-16FD02D07F5D}"/>
+    <workbookView xWindow="2910" yWindow="1395" windowWidth="19665" windowHeight="12780" xr2:uid="{645D6CBF-11AA-407D-8E7D-16FD02D07F5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -450,7 +450,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,16 +770,16 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="C15" s="7">
-        <v>1</v>
+        <v>1.0208333333333333</v>
       </c>
       <c r="D15" s="5">
         <f t="shared" si="0"/>
-        <v>0.22916666666666663</v>
+        <v>0.24999999999999989</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="8">
         <f t="shared" si="1"/>
-        <v>1.8923611111111107</v>
+        <v>1.9131944444444442</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -790,7 +790,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="8">
         <f t="shared" si="1"/>
-        <v>1.8923611111111107</v>
+        <v>1.9131944444444442</v>
       </c>
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.25">
@@ -801,7 +801,7 @@
       <c r="E17" s="4"/>
       <c r="F17" s="8">
         <f t="shared" si="1"/>
-        <v>1.8923611111111107</v>
+        <v>1.9131944444444442</v>
       </c>
     </row>
     <row r="18" spans="4:6" x14ac:dyDescent="0.25">
@@ -812,7 +812,7 @@
       <c r="E18" s="4"/>
       <c r="F18" s="8">
         <f t="shared" si="1"/>
-        <v>1.8923611111111107</v>
+        <v>1.9131944444444442</v>
       </c>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.25">
@@ -823,7 +823,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="8">
         <f t="shared" si="1"/>
-        <v>1.8923611111111107</v>
+        <v>1.9131944444444442</v>
       </c>
     </row>
     <row r="20" spans="4:6" x14ac:dyDescent="0.25">
@@ -834,7 +834,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="8">
         <f t="shared" si="1"/>
-        <v>1.8923611111111107</v>
+        <v>1.9131944444444442</v>
       </c>
     </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.25">
@@ -845,7 +845,7 @@
       <c r="E21" s="4"/>
       <c r="F21" s="8">
         <f t="shared" si="1"/>
-        <v>1.8923611111111107</v>
+        <v>1.9131944444444442</v>
       </c>
     </row>
     <row r="22" spans="4:6" x14ac:dyDescent="0.25">
@@ -855,7 +855,7 @@
       </c>
       <c r="F22" s="8">
         <f t="shared" si="1"/>
-        <v>1.8923611111111107</v>
+        <v>1.9131944444444442</v>
       </c>
     </row>
     <row r="23" spans="4:6" x14ac:dyDescent="0.25">
@@ -865,7 +865,7 @@
       </c>
       <c r="F23" s="8">
         <f t="shared" si="1"/>
-        <v>1.8923611111111107</v>
+        <v>1.9131944444444442</v>
       </c>
     </row>
     <row r="24" spans="4:6" x14ac:dyDescent="0.25">
@@ -875,7 +875,7 @@
       </c>
       <c r="F24" s="8">
         <f t="shared" si="1"/>
-        <v>1.8923611111111107</v>
+        <v>1.9131944444444442</v>
       </c>
     </row>
     <row r="25" spans="4:6" x14ac:dyDescent="0.25">
@@ -885,7 +885,7 @@
       </c>
       <c r="F25" s="8">
         <f t="shared" si="1"/>
-        <v>1.8923611111111107</v>
+        <v>1.9131944444444442</v>
       </c>
     </row>
     <row r="26" spans="4:6" x14ac:dyDescent="0.25">
@@ -895,7 +895,7 @@
       </c>
       <c r="F26" s="8">
         <f t="shared" si="1"/>
-        <v>1.8923611111111107</v>
+        <v>1.9131944444444442</v>
       </c>
     </row>
     <row r="27" spans="4:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Unity tabs + character sheet
</commit_message>
<xml_diff>
--- a/aikataulutus/Tyotunnit.xlsx
+++ b/aikataulutus/Tyotunnit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riku\Koulu\Ohjelmointyo\aikataulutus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D35942-9E42-480E-8D1C-BB2520941D3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8806F0-E97F-4575-904B-039531A5BFEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2910" yWindow="1395" windowWidth="19665" windowHeight="12780" xr2:uid="{645D6CBF-11AA-407D-8E7D-16FD02D07F5D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Paivamaara</t>
   </si>
@@ -90,6 +90,15 @@
   </si>
   <si>
     <t>database korjaus + unity UI + character info</t>
+  </si>
+  <si>
+    <t>eli verrattuna 100%</t>
+  </si>
+  <si>
+    <t>Verrataan puoleen, koska excel ei osaa maaritella isoja tunteja</t>
+  </si>
+  <si>
+    <t>Unity UI page view swap + character funktioita ja kehityksprosessin uudelleenajattelua Unity kokemuksien perusteella</t>
   </si>
 </sst>
 </file>
@@ -98,7 +107,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="174" formatCode="[h]:mm"/>
+    <numFmt numFmtId="165" formatCode="[h]:mm"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -129,13 +138,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -143,10 +149,19 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
@@ -465,7 +480,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,26 +493,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>15</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -510,22 +528,22 @@
       <c r="C2" s="2">
         <v>0.73958333333333337</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <f>C2-B2</f>
         <v>5.208333333333337E-2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="7">
         <f>D2</f>
         <v>5.208333333333337E-2</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="7">
         <f>H2-F2</f>
         <v>2.65625</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="7">
         <v>2.7083333333333335</v>
       </c>
       <c r="I2" t="s">
@@ -542,18 +560,18 @@
       <c r="C3" s="2">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D3" s="7">
-        <f t="shared" ref="D3:D41" si="0">C3-B3</f>
+      <c r="D3" s="6">
+        <f t="shared" ref="D3:D40" si="0">C3-B3</f>
         <v>0.125</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="7">
         <f>F2+D3</f>
         <v>0.17708333333333337</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="7">
         <f>H2-F3</f>
         <v>2.53125</v>
       </c>
@@ -568,18 +586,18 @@
       <c r="C4" s="2">
         <v>0.77083333333333337</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="7">
         <f>F3+D4</f>
         <v>0.30208333333333337</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="7">
         <f>H2-F4</f>
         <v>2.40625</v>
       </c>
@@ -594,18 +612,18 @@
       <c r="C5" s="2">
         <v>0.94791666666666663</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <f t="shared" si="0"/>
         <v>0.23958333333333326</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="7">
         <f t="shared" ref="F5:F26" si="1">F4+D5</f>
         <v>0.54166666666666663</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="7">
         <f>H2-F5</f>
         <v>2.166666666666667</v>
       </c>
@@ -620,18 +638,18 @@
       <c r="C6" s="2">
         <v>0.78125</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <f t="shared" si="0"/>
         <v>0.16666666666666663</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7">
         <f t="shared" si="1"/>
         <v>0.70833333333333326</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <f>H2-F6</f>
         <v>2</v>
       </c>
@@ -646,18 +664,18 @@
       <c r="C7" s="2">
         <v>7.9861111111111105E-2</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <f t="shared" si="0"/>
         <v>6.9444444444444434E-2</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="7">
         <f t="shared" si="1"/>
         <v>0.77777777777777768</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="7">
         <f>H2-F7</f>
         <v>1.9305555555555558</v>
       </c>
@@ -672,16 +690,16 @@
       <c r="C8" s="2">
         <v>1</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="6">
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="8">
+      <c r="E8" s="8"/>
+      <c r="F8" s="7">
         <f t="shared" si="1"/>
         <v>0.86111111111111105</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="7">
         <f>H2-F8</f>
         <v>1.8472222222222223</v>
       </c>
@@ -693,19 +711,19 @@
       <c r="B9" s="2">
         <v>0.91666666666666663</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>1.03125</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <f t="shared" si="0"/>
         <v>0.11458333333333337</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="8">
+      <c r="E9" s="8"/>
+      <c r="F9" s="7">
         <f t="shared" si="1"/>
         <v>0.97569444444444442</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <f>H2-F9</f>
         <v>1.7326388888888891</v>
       </c>
@@ -720,18 +738,18 @@
       <c r="C10" s="2">
         <v>0.875</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="6">
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="7">
         <f t="shared" si="1"/>
         <v>1.0590277777777777</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="7">
         <f>H2-F10</f>
         <v>1.6493055555555558</v>
       </c>
@@ -746,18 +764,18 @@
       <c r="C11" s="2">
         <v>0.97916666666666663</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="6">
         <f t="shared" si="0"/>
         <v>3.125E-2</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="7">
         <f t="shared" si="1"/>
         <v>1.0902777777777777</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="7">
         <f>H2-F11</f>
         <v>1.6180555555555558</v>
       </c>
@@ -769,21 +787,21 @@
       <c r="B12" s="2">
         <v>0.83333333333333337</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>0.97916666666666663</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <f t="shared" si="0"/>
         <v>0.14583333333333326</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="7">
         <f t="shared" si="1"/>
         <v>1.2361111111111109</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="7">
         <f>H2-F12</f>
         <v>1.4722222222222225</v>
       </c>
@@ -795,21 +813,21 @@
       <c r="B13" s="2">
         <v>0.83333333333333337</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>1.0416666666666667</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <f t="shared" si="0"/>
         <v>0.20833333333333337</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="7">
         <f t="shared" si="1"/>
         <v>1.4444444444444442</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="7">
         <f>H2-F13</f>
         <v>1.2638888888888893</v>
       </c>
@@ -821,21 +839,21 @@
       <c r="B14" s="2">
         <v>0.79166666666666663</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>1.0104166666666667</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="6">
         <f t="shared" si="0"/>
         <v>0.21875000000000011</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="7">
         <f t="shared" si="1"/>
         <v>1.6631944444444442</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="7">
         <f>H2-F14</f>
         <v>1.0451388888888893</v>
       </c>
@@ -847,288 +865,308 @@
       <c r="B15" s="2">
         <v>0.77083333333333337</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <v>1.0208333333333333</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="6">
         <f t="shared" si="0"/>
         <v>0.24999999999999989</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="7">
         <f t="shared" si="1"/>
         <v>1.9131944444444442</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="7">
         <f>H2-F15+H2</f>
         <v>3.5034722222222228</v>
       </c>
       <c r="H15" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D16" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="8">
-        <f t="shared" si="1"/>
-        <v>1.9131944444444442</v>
-      </c>
-      <c r="G16" s="8">
+      <c r="I15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>44082</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.94791666666666663</v>
+      </c>
+      <c r="D16" s="6">
+        <f t="shared" si="0"/>
+        <v>0.21875</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="7">
+        <f t="shared" si="1"/>
+        <v>2.1319444444444442</v>
+      </c>
+      <c r="G16" s="7">
         <f>H2-F16+H2</f>
-        <v>3.5034722222222228</v>
+        <v>3.2847222222222228</v>
       </c>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D17" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="8">
-        <f t="shared" si="1"/>
-        <v>1.9131944444444442</v>
-      </c>
-      <c r="G17" s="8">
+      <c r="D17" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="7">
+        <f t="shared" si="1"/>
+        <v>2.1319444444444442</v>
+      </c>
+      <c r="G17" s="7">
         <f>H2-F17+H2</f>
-        <v>3.5034722222222228</v>
+        <v>3.2847222222222228</v>
       </c>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D18" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="8">
-        <f t="shared" si="1"/>
-        <v>1.9131944444444442</v>
-      </c>
-      <c r="G18" s="8">
+      <c r="D18" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="7">
+        <f t="shared" si="1"/>
+        <v>2.1319444444444442</v>
+      </c>
+      <c r="G18" s="7">
         <f>H2-F18+H2</f>
-        <v>3.5034722222222228</v>
+        <v>3.2847222222222228</v>
       </c>
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D19" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="8">
-        <f t="shared" si="1"/>
-        <v>1.9131944444444442</v>
-      </c>
-      <c r="G19" s="8">
+      <c r="D19" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="7">
+        <f t="shared" si="1"/>
+        <v>2.1319444444444442</v>
+      </c>
+      <c r="G19" s="7">
         <f>H2-F19+H2</f>
-        <v>3.5034722222222228</v>
+        <v>3.2847222222222228</v>
       </c>
     </row>
     <row r="20" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D20" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="8">
-        <f t="shared" si="1"/>
-        <v>1.9131944444444442</v>
-      </c>
-      <c r="G20" s="8">
+      <c r="D20" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="7">
+        <f t="shared" si="1"/>
+        <v>2.1319444444444442</v>
+      </c>
+      <c r="G20" s="7">
         <f>H2-F20+H2</f>
-        <v>3.5034722222222228</v>
+        <v>3.2847222222222228</v>
       </c>
     </row>
     <row r="21" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D21" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="8">
-        <f t="shared" si="1"/>
-        <v>1.9131944444444442</v>
-      </c>
-      <c r="G21" s="8">
+      <c r="D21" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="7">
+        <f t="shared" si="1"/>
+        <v>2.1319444444444442</v>
+      </c>
+      <c r="G21" s="7">
         <f>H2-F21+H2</f>
-        <v>3.5034722222222228</v>
+        <v>3.2847222222222228</v>
       </c>
     </row>
     <row r="22" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D22" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F22" s="8">
-        <f t="shared" si="1"/>
-        <v>1.9131944444444442</v>
-      </c>
-      <c r="G22" s="8">
+      <c r="D22" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="7">
+        <f t="shared" si="1"/>
+        <v>2.1319444444444442</v>
+      </c>
+      <c r="G22" s="7">
         <f>H2-F22+H2</f>
-        <v>3.5034722222222228</v>
+        <v>3.2847222222222228</v>
       </c>
     </row>
     <row r="23" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D23" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F23" s="8">
-        <f t="shared" si="1"/>
-        <v>1.9131944444444442</v>
-      </c>
-      <c r="G23" s="8">
+      <c r="D23" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E23" s="8"/>
+      <c r="F23" s="7">
+        <f t="shared" si="1"/>
+        <v>2.1319444444444442</v>
+      </c>
+      <c r="G23" s="7">
         <f>H2-F23+H2</f>
-        <v>3.5034722222222228</v>
+        <v>3.2847222222222228</v>
       </c>
     </row>
     <row r="24" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D24" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F24" s="8">
-        <f t="shared" si="1"/>
-        <v>1.9131944444444442</v>
-      </c>
-      <c r="G24" s="8">
+      <c r="D24" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E24" s="8"/>
+      <c r="F24" s="7">
+        <f t="shared" si="1"/>
+        <v>2.1319444444444442</v>
+      </c>
+      <c r="G24" s="7">
         <f>H2-F24+H2</f>
-        <v>3.5034722222222228</v>
+        <v>3.2847222222222228</v>
       </c>
     </row>
     <row r="25" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D25" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="8">
-        <f t="shared" si="1"/>
-        <v>1.9131944444444442</v>
-      </c>
-      <c r="G25" s="8">
+      <c r="D25" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E25" s="8"/>
+      <c r="F25" s="7">
+        <f t="shared" si="1"/>
+        <v>2.1319444444444442</v>
+      </c>
+      <c r="G25" s="7">
         <f>H2-F25+H2</f>
-        <v>3.5034722222222228</v>
+        <v>3.2847222222222228</v>
       </c>
     </row>
     <row r="26" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D26" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F26" s="8">
-        <f t="shared" si="1"/>
-        <v>1.9131944444444442</v>
-      </c>
-      <c r="G26" s="8">
+      <c r="D26" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E26" s="8"/>
+      <c r="F26" s="7">
+        <f t="shared" si="1"/>
+        <v>2.1319444444444442</v>
+      </c>
+      <c r="G26" s="7">
         <f>H2-F26+H2</f>
-        <v>3.5034722222222228</v>
+        <v>3.2847222222222228</v>
       </c>
     </row>
     <row r="27" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D27" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
+      <c r="D27" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E27" s="8"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
     </row>
     <row r="28" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D28" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F28" s="8"/>
+      <c r="D28" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="7"/>
     </row>
     <row r="29" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D29" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F29" s="8"/>
+      <c r="D29" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="7"/>
     </row>
     <row r="30" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D30" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F30" s="8"/>
+      <c r="D30" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="7"/>
     </row>
     <row r="31" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D31" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F31" s="8"/>
+      <c r="D31" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="7"/>
     </row>
     <row r="32" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D32" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F32" s="8"/>
+      <c r="D32" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="7"/>
     </row>
     <row r="33" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D33" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F33" s="8"/>
+      <c r="D33" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F33" s="7"/>
     </row>
     <row r="34" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D34" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F34" s="8"/>
+      <c r="D34" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="7"/>
     </row>
     <row r="35" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D35" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F35" s="8"/>
+      <c r="D35" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F35" s="7"/>
     </row>
     <row r="36" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D36" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F36" s="8"/>
+      <c r="D36" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F36" s="7"/>
     </row>
     <row r="37" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D37" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F37" s="8"/>
+      <c r="D37" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F37" s="7"/>
     </row>
     <row r="38" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D38" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F38" s="8"/>
+      <c r="D38" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F38" s="7"/>
     </row>
     <row r="39" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D39" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F39" s="8"/>
+      <c r="D39" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F39" s="7"/>
     </row>
     <row r="40" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D40" s="7">
+      <c r="D40" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D41" s="5"/>
+      <c r="D41" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
XML dictionary luonti toimii
</commit_message>
<xml_diff>
--- a/aikataulutus/Tyotunnit.xlsx
+++ b/aikataulutus/Tyotunnit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riku\Koulu\Ohjelmointyo\aikataulutus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8CA68B-706F-4F0A-9CF0-4C269D1F40EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD275888-869C-48E3-9651-C6E89789CC80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2910" yWindow="1395" windowWidth="19665" windowHeight="12780" xr2:uid="{645D6CBF-11AA-407D-8E7D-16FD02D07F5D}"/>
   </bookViews>
@@ -483,7 +483,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,18 +946,27 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>44084</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.91666666666666663</v>
+      </c>
       <c r="D18" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.20833333333333326</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="7">
         <f t="shared" si="1"/>
-        <v>2.2986111111111107</v>
+        <v>2.5069444444444438</v>
       </c>
       <c r="G18" s="7">
         <f>H2-F18+H2</f>
-        <v>3.1180555555555562</v>
+        <v>2.9097222222222232</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -968,11 +977,11 @@
       <c r="E19" s="8"/>
       <c r="F19" s="7">
         <f t="shared" si="1"/>
-        <v>2.2986111111111107</v>
+        <v>2.5069444444444438</v>
       </c>
       <c r="G19" s="7">
         <f>H2-F19+H2</f>
-        <v>3.1180555555555562</v>
+        <v>2.9097222222222232</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -983,11 +992,11 @@
       <c r="E20" s="8"/>
       <c r="F20" s="7">
         <f t="shared" si="1"/>
-        <v>2.2986111111111107</v>
+        <v>2.5069444444444438</v>
       </c>
       <c r="G20" s="7">
         <f>H2-F20+H2</f>
-        <v>3.1180555555555562</v>
+        <v>2.9097222222222232</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -998,11 +1007,11 @@
       <c r="E21" s="8"/>
       <c r="F21" s="7">
         <f t="shared" si="1"/>
-        <v>2.2986111111111107</v>
+        <v>2.5069444444444438</v>
       </c>
       <c r="G21" s="7">
         <f>H2-F21+H2</f>
-        <v>3.1180555555555562</v>
+        <v>2.9097222222222232</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1013,11 +1022,11 @@
       <c r="E22" s="8"/>
       <c r="F22" s="7">
         <f t="shared" si="1"/>
-        <v>2.2986111111111107</v>
+        <v>2.5069444444444438</v>
       </c>
       <c r="G22" s="7">
         <f>H2-F22+H2</f>
-        <v>3.1180555555555562</v>
+        <v>2.9097222222222232</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1028,11 +1037,11 @@
       <c r="E23" s="8"/>
       <c r="F23" s="7">
         <f t="shared" si="1"/>
-        <v>2.2986111111111107</v>
+        <v>2.5069444444444438</v>
       </c>
       <c r="G23" s="7">
         <f>H2-F23+H2</f>
-        <v>3.1180555555555562</v>
+        <v>2.9097222222222232</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1043,11 +1052,11 @@
       <c r="E24" s="8"/>
       <c r="F24" s="7">
         <f t="shared" si="1"/>
-        <v>2.2986111111111107</v>
+        <v>2.5069444444444438</v>
       </c>
       <c r="G24" s="7">
         <f>H2-F24+H2</f>
-        <v>3.1180555555555562</v>
+        <v>2.9097222222222232</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1058,11 +1067,11 @@
       <c r="E25" s="8"/>
       <c r="F25" s="7">
         <f t="shared" si="1"/>
-        <v>2.2986111111111107</v>
+        <v>2.5069444444444438</v>
       </c>
       <c r="G25" s="7">
         <f>H2-F25+H2</f>
-        <v>3.1180555555555562</v>
+        <v>2.9097222222222232</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1073,11 +1082,11 @@
       <c r="E26" s="8"/>
       <c r="F26" s="7">
         <f t="shared" si="1"/>
-        <v>2.2986111111111107</v>
+        <v>2.5069444444444438</v>
       </c>
       <c r="G26" s="7">
         <f>H2-F26+H2</f>
-        <v>3.1180555555555562</v>
+        <v>2.9097222222222232</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
XMLParse, UI from Character, Character creation, Character Class
XMLParse:
- dictionaryt toimivia ja loopissa.

UI from Character:
- staattisen siirron sijaan, tieto tulee Character luokasta.

Character Creation:
- Kehitetaan tiedonsaanti dictionareista ja luodaan hallinnointi metodeja.

Character Class
- Muutetaan tiedot internal muotoon.
</commit_message>
<xml_diff>
--- a/aikataulutus/Tyotunnit.xlsx
+++ b/aikataulutus/Tyotunnit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riku\Koulu\Ohjelmointyo\aikataulutus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD275888-869C-48E3-9651-C6E89789CC80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A5CC67-7AF3-43BA-BE02-DE20F5B2AEEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2910" yWindow="1395" windowWidth="19665" windowHeight="12780" xr2:uid="{645D6CBF-11AA-407D-8E7D-16FD02D07F5D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Paivamaara</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>XML parset luotu ja  looped, manuaalisen sijaan (ensin KAIKKI manuaaliset rakennettu, jotka myohemmin loopattu, johon meni turhaan aikaa) + comments (harkintaa progression dictionarien looppaamisesta)</t>
+  </si>
+  <si>
+    <t>XMLParse korjattu (dictionarit valmiina). Character creation rakennettu internal ja tiedot characterista UI, staattisen tiedon sijaan</t>
   </si>
 </sst>
 </file>
@@ -482,8 +485,8 @@
   <sheetPr codeName="Taul1"/>
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,7 +948,7 @@
         <v>3.1180555555555562</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44084</v>
       </c>
@@ -959,7 +962,9 @@
         <f t="shared" si="0"/>
         <v>0.20833333333333326</v>
       </c>
-      <c r="E18" s="8"/>
+      <c r="E18" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="F18" s="7">
         <f t="shared" si="1"/>
         <v>2.5069444444444438</v>

</xml_diff>

<commit_message>
Skill Increase + Character Advancement
Skill Increase
- works

Character Advancement
- Can add feats and advancements (no filter)
- Will have to change XML format or dictionary keys?
</commit_message>
<xml_diff>
--- a/aikataulutus/Tyotunnit.xlsx
+++ b/aikataulutus/Tyotunnit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riku\Koulu\Ohjelmointyo\aikataulutus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A5CC67-7AF3-43BA-BE02-DE20F5B2AEEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410C4726-92DB-4682-83EB-FB4E7EFCFC12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2910" yWindow="1395" windowWidth="19665" windowHeight="12780" xr2:uid="{645D6CBF-11AA-407D-8E7D-16FD02D07F5D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Paivamaara</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>XMLParse korjattu (dictionarit valmiina). Character creation rakennettu internal ja tiedot characterista UI, staattisen tiedon sijaan</t>
+  </si>
+  <si>
+    <t>Skill Increase + Character Advancement</t>
   </si>
 </sst>
 </file>
@@ -486,7 +489,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -975,18 +978,29 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>44085</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.33333333333333331</v>
+      </c>
       <c r="D19" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E19" s="8"/>
+        <v>8.3333333333333315E-2</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="F19" s="7">
         <f t="shared" si="1"/>
-        <v>2.5069444444444438</v>
+        <v>2.5902777777777772</v>
       </c>
       <c r="G19" s="7">
         <f>H2-F19+H2</f>
-        <v>2.9097222222222232</v>
+        <v>2.8263888888888897</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -997,11 +1011,11 @@
       <c r="E20" s="8"/>
       <c r="F20" s="7">
         <f t="shared" si="1"/>
-        <v>2.5069444444444438</v>
+        <v>2.5902777777777772</v>
       </c>
       <c r="G20" s="7">
         <f>H2-F20+H2</f>
-        <v>2.9097222222222232</v>
+        <v>2.8263888888888897</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1012,11 +1026,11 @@
       <c r="E21" s="8"/>
       <c r="F21" s="7">
         <f t="shared" si="1"/>
-        <v>2.5069444444444438</v>
+        <v>2.5902777777777772</v>
       </c>
       <c r="G21" s="7">
         <f>H2-F21+H2</f>
-        <v>2.9097222222222232</v>
+        <v>2.8263888888888897</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1027,11 +1041,11 @@
       <c r="E22" s="8"/>
       <c r="F22" s="7">
         <f t="shared" si="1"/>
-        <v>2.5069444444444438</v>
+        <v>2.5902777777777772</v>
       </c>
       <c r="G22" s="7">
         <f>H2-F22+H2</f>
-        <v>2.9097222222222232</v>
+        <v>2.8263888888888897</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1042,11 +1056,11 @@
       <c r="E23" s="8"/>
       <c r="F23" s="7">
         <f t="shared" si="1"/>
-        <v>2.5069444444444438</v>
+        <v>2.5902777777777772</v>
       </c>
       <c r="G23" s="7">
         <f>H2-F23+H2</f>
-        <v>2.9097222222222232</v>
+        <v>2.8263888888888897</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1057,11 +1071,11 @@
       <c r="E24" s="8"/>
       <c r="F24" s="7">
         <f t="shared" si="1"/>
-        <v>2.5069444444444438</v>
+        <v>2.5902777777777772</v>
       </c>
       <c r="G24" s="7">
         <f>H2-F24+H2</f>
-        <v>2.9097222222222232</v>
+        <v>2.8263888888888897</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1072,11 +1086,11 @@
       <c r="E25" s="8"/>
       <c r="F25" s="7">
         <f t="shared" si="1"/>
-        <v>2.5069444444444438</v>
+        <v>2.5902777777777772</v>
       </c>
       <c r="G25" s="7">
         <f>H2-F25+H2</f>
-        <v>2.9097222222222232</v>
+        <v>2.8263888888888897</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1087,11 +1101,11 @@
       <c r="E26" s="8"/>
       <c r="F26" s="7">
         <f t="shared" si="1"/>
-        <v>2.5069444444444438</v>
+        <v>2.5902777777777772</v>
       </c>
       <c r="G26" s="7">
         <f>H2-F26+H2</f>
-        <v>2.9097222222222232</v>
+        <v>2.8263888888888897</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Revert "Revert "Add Feat""
This reverts commit 21ba9473039b9db1ab638bd59d07d78114d5eb9a.
</commit_message>
<xml_diff>
--- a/aikataulutus/Tyotunnit.xlsx
+++ b/aikataulutus/Tyotunnit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riku\Koulu\Ohjelmointyo\aikataulutus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170B5511-83D0-4BFB-A470-4746DF8FDD55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8AC319-95DA-4164-B140-56DE500AC62D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2910" yWindow="1395" windowWidth="19665" windowHeight="12780" xr2:uid="{645D6CBF-11AA-407D-8E7D-16FD02D07F5D}"/>
   </bookViews>
@@ -110,7 +110,7 @@
     <t>Skill Increase + Character Advancement</t>
   </si>
   <si>
-    <t>XML + Add Advancement</t>
+    <t>XML + Add Advancement, Feats being added with partial filter</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,7 +1006,7 @@
         <v>2.8263888888888897</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44085</v>
       </c>
@@ -1014,22 +1014,22 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="C20" s="2">
-        <v>0.91666666666666663</v>
+        <v>0.98958333333333337</v>
       </c>
       <c r="D20" s="6">
         <f t="shared" si="0"/>
-        <v>0.125</v>
-      </c>
-      <c r="E20" s="8" t="s">
+        <v>0.19791666666666674</v>
+      </c>
+      <c r="E20" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F20" s="7">
         <f t="shared" si="1"/>
-        <v>2.7152777777777772</v>
+        <v>2.7881944444444438</v>
       </c>
       <c r="G20" s="7">
         <f>H2-F20+H2</f>
-        <v>2.7013888888888897</v>
+        <v>2.6284722222222232</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1040,11 +1040,11 @@
       <c r="E21" s="8"/>
       <c r="F21" s="7">
         <f t="shared" si="1"/>
-        <v>2.7152777777777772</v>
+        <v>2.7881944444444438</v>
       </c>
       <c r="G21" s="7">
         <f>H2-F21+H2</f>
-        <v>2.7013888888888897</v>
+        <v>2.6284722222222232</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1055,11 +1055,11 @@
       <c r="E22" s="8"/>
       <c r="F22" s="7">
         <f t="shared" si="1"/>
-        <v>2.7152777777777772</v>
+        <v>2.7881944444444438</v>
       </c>
       <c r="G22" s="7">
         <f>H2-F22+H2</f>
-        <v>2.7013888888888897</v>
+        <v>2.6284722222222232</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1070,11 +1070,11 @@
       <c r="E23" s="8"/>
       <c r="F23" s="7">
         <f t="shared" si="1"/>
-        <v>2.7152777777777772</v>
+        <v>2.7881944444444438</v>
       </c>
       <c r="G23" s="7">
         <f>H2-F23+H2</f>
-        <v>2.7013888888888897</v>
+        <v>2.6284722222222232</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1085,11 +1085,11 @@
       <c r="E24" s="8"/>
       <c r="F24" s="7">
         <f t="shared" si="1"/>
-        <v>2.7152777777777772</v>
+        <v>2.7881944444444438</v>
       </c>
       <c r="G24" s="7">
         <f>H2-F24+H2</f>
-        <v>2.7013888888888897</v>
+        <v>2.6284722222222232</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1100,11 +1100,11 @@
       <c r="E25" s="8"/>
       <c r="F25" s="7">
         <f t="shared" si="1"/>
-        <v>2.7152777777777772</v>
+        <v>2.7881944444444438</v>
       </c>
       <c r="G25" s="7">
         <f>H2-F25+H2</f>
-        <v>2.7013888888888897</v>
+        <v>2.6284722222222232</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1115,11 +1115,11 @@
       <c r="E26" s="8"/>
       <c r="F26" s="7">
         <f t="shared" si="1"/>
-        <v>2.7152777777777772</v>
+        <v>2.7881944444444438</v>
       </c>
       <c r="G26" s="7">
         <f>H2-F26+H2</f>
-        <v>2.7013888888888897</v>
+        <v>2.6284722222222232</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
XML + Stats + Requirement
XML
- mallinkorjaus

Stats
- muutettu dictionary muotoon parempaa käsittelyä varten, samalla kaikki metodit muutettu sopimaan dictionarylle (käytetään metodeja statistiikkojen muutokseen)

Requirement:
- Uudelleensuunniteltu miten kehitysvaatimuksia käsitellään. Aloitettu rakentamaan tulkkia kun muotona:
tarkentaja|vaatimus

- vaatii OR ja AND splittaus metodin ennen CheckRequirement metodia, eli controller metodin, joka palauttaa kehitykselle boolean arvon
</commit_message>
<xml_diff>
--- a/aikataulutus/Tyotunnit.xlsx
+++ b/aikataulutus/Tyotunnit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riku\Koulu\Ohjelmointyo\aikataulutus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E582C9E-FEF7-46C8-8F1A-93D42BB08F3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC64CF0-1C41-472E-9207-FDFBF294A967}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2910" yWindow="1395" windowWidth="19665" windowHeight="12780" xr2:uid="{645D6CBF-11AA-407D-8E7D-16FD02D07F5D}"/>
   </bookViews>
@@ -495,7 +495,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add Advancement + XML Progression
- Add Advancement lisää kaikki prerequirements avulla, jättäen pois Feat(Initial) -kategorian.

- Aikaisemmat filteröintitavat siivottu pois.

- Feat(Initial) lisätään RandomClass ja RandomAncestryn kautta, koska ne valitaan classin tai ancestryn valinnan alussa.

- XML Progression editoitu yhteensopivaksi XML Advancement kanssa.
</commit_message>
<xml_diff>
--- a/aikataulutus/Tyotunnit.xlsx
+++ b/aikataulutus/Tyotunnit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riku\Koulu\Ohjelmointyo\aikataulutus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC64CF0-1C41-472E-9207-FDFBF294A967}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820E0CBD-420C-4DCE-A0E2-DEDF3CC75BB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2910" yWindow="1395" windowWidth="19665" windowHeight="12780" xr2:uid="{645D6CBF-11AA-407D-8E7D-16FD02D07F5D}"/>
   </bookViews>
@@ -495,7 +495,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,18 +1062,27 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>44087</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.875</v>
+      </c>
       <c r="D22" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.20833333333333337</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="7">
         <f t="shared" si="1"/>
-        <v>2.9999999999999991</v>
+        <v>3.2083333333333326</v>
       </c>
       <c r="G22" s="7">
         <f>H2-F22+H2</f>
-        <v>2.4166666666666679</v>
+        <v>2.2083333333333344</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1084,11 +1093,11 @@
       <c r="E23" s="8"/>
       <c r="F23" s="7">
         <f t="shared" si="1"/>
-        <v>2.9999999999999991</v>
+        <v>3.2083333333333326</v>
       </c>
       <c r="G23" s="7">
         <f>H2-F23+H2</f>
-        <v>2.4166666666666679</v>
+        <v>2.2083333333333344</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1099,11 +1108,11 @@
       <c r="E24" s="8"/>
       <c r="F24" s="7">
         <f t="shared" si="1"/>
-        <v>2.9999999999999991</v>
+        <v>3.2083333333333326</v>
       </c>
       <c r="G24" s="7">
         <f>H2-F24+H2</f>
-        <v>2.4166666666666679</v>
+        <v>2.2083333333333344</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1114,11 +1123,11 @@
       <c r="E25" s="8"/>
       <c r="F25" s="7">
         <f t="shared" si="1"/>
-        <v>2.9999999999999991</v>
+        <v>3.2083333333333326</v>
       </c>
       <c r="G25" s="7">
         <f>H2-F25+H2</f>
-        <v>2.4166666666666679</v>
+        <v>2.2083333333333344</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1129,11 +1138,11 @@
       <c r="E26" s="8"/>
       <c r="F26" s="7">
         <f t="shared" si="1"/>
-        <v>2.9999999999999991</v>
+        <v>3.2083333333333326</v>
       </c>
       <c r="G26" s="7">
         <f>H2-F26+H2</f>
-        <v>2.4166666666666679</v>
+        <v>2.2083333333333344</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Skill Increase bugfix + XML format + Character features + Documentation
Skill Increase bugfix:
- uusi randomgen skill jos kyseinen skill on jo maksimitasossa, tuotti index errorin.
- System.Random ei ole täysin random, vaan perustuu random arvoon joka generoidaan tietyksi ajaksi, joten saatetaan tehdä erillinen metodi tämän välttämiseksi optimointia varten.

XML format:
- XML tiedostojen formatointia sopimaan ohjelman dictionareihin

Character features:
- hp, size, ym. määritelty hahmolle myöhempää käyttöä varten

Documentation:
Dokumentaation päivitystä omista muistiinpanoista ja huomioista
</commit_message>
<xml_diff>
--- a/aikataulutus/Tyotunnit.xlsx
+++ b/aikataulutus/Tyotunnit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riku\Koulu\Ohjelmointyo\aikataulutus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820E0CBD-420C-4DCE-A0E2-DEDF3CC75BB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022B563A-AC8C-49EA-89D6-A05E4725F238}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2910" yWindow="1395" windowWidth="19665" windowHeight="12780" xr2:uid="{645D6CBF-11AA-407D-8E7D-16FD02D07F5D}"/>
   </bookViews>
@@ -1069,20 +1069,20 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C22" s="2">
-        <v>0.875</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="D22" s="6">
         <f t="shared" si="0"/>
-        <v>0.20833333333333337</v>
+        <v>0.25</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="7">
         <f t="shared" si="1"/>
-        <v>3.2083333333333326</v>
+        <v>3.2499999999999991</v>
       </c>
       <c r="G22" s="7">
         <f>H2-F22+H2</f>
-        <v>2.2083333333333344</v>
+        <v>2.1666666666666679</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1093,11 +1093,11 @@
       <c r="E23" s="8"/>
       <c r="F23" s="7">
         <f t="shared" si="1"/>
-        <v>3.2083333333333326</v>
+        <v>3.2499999999999991</v>
       </c>
       <c r="G23" s="7">
         <f>H2-F23+H2</f>
-        <v>2.2083333333333344</v>
+        <v>2.1666666666666679</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1108,11 +1108,11 @@
       <c r="E24" s="8"/>
       <c r="F24" s="7">
         <f t="shared" si="1"/>
-        <v>3.2083333333333326</v>
+        <v>3.2499999999999991</v>
       </c>
       <c r="G24" s="7">
         <f>H2-F24+H2</f>
-        <v>2.2083333333333344</v>
+        <v>2.1666666666666679</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1123,11 +1123,11 @@
       <c r="E25" s="8"/>
       <c r="F25" s="7">
         <f t="shared" si="1"/>
-        <v>3.2083333333333326</v>
+        <v>3.2499999999999991</v>
       </c>
       <c r="G25" s="7">
         <f>H2-F25+H2</f>
-        <v>2.2083333333333344</v>
+        <v>2.1666666666666679</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1138,11 +1138,11 @@
       <c r="E26" s="8"/>
       <c r="F26" s="7">
         <f t="shared" si="1"/>
-        <v>3.2083333333333326</v>
+        <v>3.2499999999999991</v>
       </c>
       <c r="G26" s="7">
         <f>H2-F26+H2</f>
-        <v>2.2083333333333344</v>
+        <v>2.1666666666666679</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Apply background, ancestry, proficiencies
- Feat Assurance() ongelman välttämistä, jota yritetään ratkaista sattumanvaraisen ja tarkennetun valinnan aikana.
- Jokaisen kolmen XML tiedoston läpikäyntiä oikeaan formatointiin ja käsittelyyn
- background melkein valmis (feat Assurance ongelma)
</commit_message>
<xml_diff>
--- a/aikataulutus/Tyotunnit.xlsx
+++ b/aikataulutus/Tyotunnit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riku\Koulu\Ohjelmointyo\aikataulutus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A399671-90FC-4712-91FD-58D74B00B4B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CACCDA94-F582-4A21-BDD8-43C029309397}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2910" yWindow="1395" windowWidth="19665" windowHeight="12780" xr2:uid="{645D6CBF-11AA-407D-8E7D-16FD02D07F5D}"/>
   </bookViews>
@@ -498,7 +498,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,20 +1098,20 @@
         <v>0.67708333333333337</v>
       </c>
       <c r="C23" s="2">
-        <v>0.88541666666666663</v>
+        <v>0.89583333333333337</v>
       </c>
       <c r="D23" s="6">
         <f t="shared" si="0"/>
-        <v>0.20833333333333326</v>
+        <v>0.21875</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="7">
         <f t="shared" si="1"/>
-        <v>3.4583333333333321</v>
+        <v>3.4687499999999991</v>
       </c>
       <c r="G23" s="7">
         <f>H2-F23+H2</f>
-        <v>1.9583333333333348</v>
+        <v>1.9479166666666679</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1122,11 +1122,11 @@
       <c r="E24" s="8"/>
       <c r="F24" s="7">
         <f t="shared" si="1"/>
-        <v>3.4583333333333321</v>
+        <v>3.4687499999999991</v>
       </c>
       <c r="G24" s="7">
         <f>H2-F24+H2</f>
-        <v>1.9583333333333348</v>
+        <v>1.9479166666666679</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1137,11 +1137,11 @@
       <c r="E25" s="8"/>
       <c r="F25" s="7">
         <f t="shared" si="1"/>
-        <v>3.4583333333333321</v>
+        <v>3.4687499999999991</v>
       </c>
       <c r="G25" s="7">
         <f>H2-F25+H2</f>
-        <v>1.9583333333333348</v>
+        <v>1.9479166666666679</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1152,11 +1152,11 @@
       <c r="E26" s="8"/>
       <c r="F26" s="7">
         <f t="shared" si="1"/>
-        <v>3.4583333333333321</v>
+        <v>3.4687499999999991</v>
       </c>
       <c r="G26" s="7">
         <f>H2-F26+H2</f>
-        <v>1.9583333333333348</v>
+        <v>1.9479166666666679</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1167,11 +1167,11 @@
       <c r="E27" s="8"/>
       <c r="F27" s="7">
         <f t="shared" si="1"/>
-        <v>3.4583333333333321</v>
+        <v>3.4687499999999991</v>
       </c>
       <c r="G27" s="7">
         <f>H2-F27+H2</f>
-        <v>1.9583333333333348</v>
+        <v>1.9479166666666679</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1181,11 +1181,11 @@
       </c>
       <c r="F28" s="7">
         <f t="shared" si="1"/>
-        <v>3.4583333333333321</v>
+        <v>3.4687499999999991</v>
       </c>
       <c r="G28" s="7">
         <f>H2-F28+H2</f>
-        <v>1.9583333333333348</v>
+        <v>1.9479166666666679</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1195,11 +1195,11 @@
       </c>
       <c r="F29" s="7">
         <f t="shared" si="1"/>
-        <v>3.4583333333333321</v>
+        <v>3.4687499999999991</v>
       </c>
       <c r="G29" s="7">
         <f>H2-F29+H2</f>
-        <v>1.9583333333333348</v>
+        <v>1.9479166666666679</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1209,11 +1209,11 @@
       </c>
       <c r="F30" s="7">
         <f t="shared" si="1"/>
-        <v>3.4583333333333321</v>
+        <v>3.4687499999999991</v>
       </c>
       <c r="G30" s="7">
         <f>H2-F30+H2</f>
-        <v>1.9583333333333348</v>
+        <v>1.9479166666666679</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1223,11 +1223,11 @@
       </c>
       <c r="F31" s="7">
         <f t="shared" si="1"/>
-        <v>3.4583333333333321</v>
+        <v>3.4687499999999991</v>
       </c>
       <c r="G31" s="7">
         <f>H2-F31+H2</f>
-        <v>1.9583333333333348</v>
+        <v>1.9479166666666679</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1237,11 +1237,11 @@
       </c>
       <c r="F32" s="7">
         <f t="shared" si="1"/>
-        <v>3.4583333333333321</v>
+        <v>3.4687499999999991</v>
       </c>
       <c r="G32" s="7">
         <f>H2-F32+H2</f>
-        <v>1.9583333333333348</v>
+        <v>1.9479166666666679</v>
       </c>
     </row>
     <row r="33" spans="4:7" x14ac:dyDescent="0.25">
@@ -1251,11 +1251,11 @@
       </c>
       <c r="F33" s="7">
         <f t="shared" si="1"/>
-        <v>3.4583333333333321</v>
+        <v>3.4687499999999991</v>
       </c>
       <c r="G33" s="7">
         <f>H2-F33+H2</f>
-        <v>1.9583333333333348</v>
+        <v>1.9479166666666679</v>
       </c>
     </row>
     <row r="34" spans="4:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Apply background, Apply ancestries
Apply background, ancestries:
- toimivat

BUG:
- Monk Class Feats = 0, (proficiencies?)
- Champion  Class Feats = 0, (proficiencies?)
</commit_message>
<xml_diff>
--- a/aikataulutus/Tyotunnit.xlsx
+++ b/aikataulutus/Tyotunnit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riku\Koulu\Ohjelmointyo\aikataulutus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CACCDA94-F582-4A21-BDD8-43C029309397}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ADA85DB-0AFE-4571-91AC-747E4D63BD48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2910" yWindow="1395" windowWidth="19665" windowHeight="12780" xr2:uid="{645D6CBF-11AA-407D-8E7D-16FD02D07F5D}"/>
   </bookViews>
@@ -497,8 +497,8 @@
   <sheetPr codeName="Taul1"/>
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,18 +1115,27 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>44089</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.89583333333333337</v>
+      </c>
       <c r="D24" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.20833333333333337</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="7">
         <f t="shared" si="1"/>
-        <v>3.4687499999999991</v>
+        <v>3.6770833333333326</v>
       </c>
       <c r="G24" s="7">
         <f>H2-F24+H2</f>
-        <v>1.9479166666666679</v>
+        <v>1.7395833333333344</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1137,11 +1146,11 @@
       <c r="E25" s="8"/>
       <c r="F25" s="7">
         <f t="shared" si="1"/>
-        <v>3.4687499999999991</v>
+        <v>3.6770833333333326</v>
       </c>
       <c r="G25" s="7">
         <f>H2-F25+H2</f>
-        <v>1.9479166666666679</v>
+        <v>1.7395833333333344</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1152,11 +1161,11 @@
       <c r="E26" s="8"/>
       <c r="F26" s="7">
         <f t="shared" si="1"/>
-        <v>3.4687499999999991</v>
+        <v>3.6770833333333326</v>
       </c>
       <c r="G26" s="7">
         <f>H2-F26+H2</f>
-        <v>1.9479166666666679</v>
+        <v>1.7395833333333344</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1167,11 +1176,11 @@
       <c r="E27" s="8"/>
       <c r="F27" s="7">
         <f t="shared" si="1"/>
-        <v>3.4687499999999991</v>
+        <v>3.6770833333333326</v>
       </c>
       <c r="G27" s="7">
         <f>H2-F27+H2</f>
-        <v>1.9479166666666679</v>
+        <v>1.7395833333333344</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1181,11 +1190,11 @@
       </c>
       <c r="F28" s="7">
         <f t="shared" si="1"/>
-        <v>3.4687499999999991</v>
+        <v>3.6770833333333326</v>
       </c>
       <c r="G28" s="7">
         <f>H2-F28+H2</f>
-        <v>1.9479166666666679</v>
+        <v>1.7395833333333344</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1195,11 +1204,11 @@
       </c>
       <c r="F29" s="7">
         <f t="shared" si="1"/>
-        <v>3.4687499999999991</v>
+        <v>3.6770833333333326</v>
       </c>
       <c r="G29" s="7">
         <f>H2-F29+H2</f>
-        <v>1.9479166666666679</v>
+        <v>1.7395833333333344</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1209,11 +1218,11 @@
       </c>
       <c r="F30" s="7">
         <f t="shared" si="1"/>
-        <v>3.4687499999999991</v>
+        <v>3.6770833333333326</v>
       </c>
       <c r="G30" s="7">
         <f>H2-F30+H2</f>
-        <v>1.9479166666666679</v>
+        <v>1.7395833333333344</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1223,11 +1232,11 @@
       </c>
       <c r="F31" s="7">
         <f t="shared" si="1"/>
-        <v>3.4687499999999991</v>
+        <v>3.6770833333333326</v>
       </c>
       <c r="G31" s="7">
         <f>H2-F31+H2</f>
-        <v>1.9479166666666679</v>
+        <v>1.7395833333333344</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1237,11 +1246,11 @@
       </c>
       <c r="F32" s="7">
         <f t="shared" si="1"/>
-        <v>3.4687499999999991</v>
+        <v>3.6770833333333326</v>
       </c>
       <c r="G32" s="7">
         <f>H2-F32+H2</f>
-        <v>1.9479166666666679</v>
+        <v>1.7395833333333344</v>
       </c>
     </row>
     <row r="33" spans="4:7" x14ac:dyDescent="0.25">
@@ -1251,11 +1260,11 @@
       </c>
       <c r="F33" s="7">
         <f t="shared" si="1"/>
-        <v>3.4687499999999991</v>
+        <v>3.6770833333333326</v>
       </c>
       <c r="G33" s="7">
         <f>H2-F33+H2</f>
-        <v>1.9479166666666679</v>
+        <v>1.7395833333333344</v>
       </c>
     </row>
     <row r="34" spans="4:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Suunnittelu + Initial Feat fix + RandomGen Tuning
BUGFIX:
- Initial feat ei aina valittu

Suunnittelu:
- README ohjelmointi kansiossa 16.9

RandomGen:
- korjattiin toimimaan paremmin randomgen stateille, todennakoisesti kokeillaan Unityn omaa Random.Range(), jotta tuottaisi aina uniikkeja (yksi level tällä hetkella on 30+ nanosekuntia vähintään system.sleep?)
</commit_message>
<xml_diff>
--- a/aikataulutus/Tyotunnit.xlsx
+++ b/aikataulutus/Tyotunnit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riku\Koulu\Ohjelmointyo\aikataulutus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97BB0DD-EC00-452F-B05C-3C524CE56DB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2A6B5E-A9DD-4B75-A71B-2A3DF263640E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2910" yWindow="1395" windowWidth="19665" windowHeight="12780" xr2:uid="{645D6CBF-11AA-407D-8E7D-16FD02D07F5D}"/>
   </bookViews>
@@ -119,7 +119,7 @@
     <t>requirements + bug fixes + documentation + XML</t>
   </si>
   <si>
-    <t>proficiencies + levelup (main stat weight)</t>
+    <t>proficiencies + levelup (main stat weight) + BUGFIX + suunnittelua(1h?)</t>
   </si>
 </sst>
 </file>
@@ -500,7 +500,7 @@
   <sheetPr codeName="Taul1"/>
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -1141,7 +1141,7 @@
         <v>1.7395833333333344</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44090</v>
       </c>
@@ -1149,22 +1149,22 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="C25" s="2">
-        <v>0.77083333333333337</v>
+        <v>0.85416666666666663</v>
       </c>
       <c r="D25" s="6">
         <f t="shared" si="0"/>
-        <v>0.125</v>
-      </c>
-      <c r="E25" s="8" t="s">
+        <v>0.20833333333333326</v>
+      </c>
+      <c r="E25" s="9" t="s">
         <v>28</v>
       </c>
       <c r="F25" s="7">
         <f t="shared" si="1"/>
-        <v>3.8020833333333326</v>
+        <v>3.8854166666666661</v>
       </c>
       <c r="G25" s="7">
         <f>H2-F25+H2</f>
-        <v>1.6145833333333344</v>
+        <v>1.5312500000000009</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1175,11 +1175,11 @@
       <c r="E26" s="8"/>
       <c r="F26" s="7">
         <f t="shared" si="1"/>
-        <v>3.8020833333333326</v>
+        <v>3.8854166666666661</v>
       </c>
       <c r="G26" s="7">
         <f>H2-F26+H2</f>
-        <v>1.6145833333333344</v>
+        <v>1.5312500000000009</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1190,11 +1190,11 @@
       <c r="E27" s="8"/>
       <c r="F27" s="7">
         <f t="shared" si="1"/>
-        <v>3.8020833333333326</v>
+        <v>3.8854166666666661</v>
       </c>
       <c r="G27" s="7">
         <f>H2-F27+H2</f>
-        <v>1.6145833333333344</v>
+        <v>1.5312500000000009</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1204,11 +1204,11 @@
       </c>
       <c r="F28" s="7">
         <f t="shared" si="1"/>
-        <v>3.8020833333333326</v>
+        <v>3.8854166666666661</v>
       </c>
       <c r="G28" s="7">
         <f>H2-F28+H2</f>
-        <v>1.6145833333333344</v>
+        <v>1.5312500000000009</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1218,11 +1218,11 @@
       </c>
       <c r="F29" s="7">
         <f t="shared" si="1"/>
-        <v>3.8020833333333326</v>
+        <v>3.8854166666666661</v>
       </c>
       <c r="G29" s="7">
         <f>H2-F29+H2</f>
-        <v>1.6145833333333344</v>
+        <v>1.5312500000000009</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1232,11 +1232,11 @@
       </c>
       <c r="F30" s="7">
         <f t="shared" si="1"/>
-        <v>3.8020833333333326</v>
+        <v>3.8854166666666661</v>
       </c>
       <c r="G30" s="7">
         <f>H2-F30+H2</f>
-        <v>1.6145833333333344</v>
+        <v>1.5312500000000009</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1246,11 +1246,11 @@
       </c>
       <c r="F31" s="7">
         <f t="shared" si="1"/>
-        <v>3.8020833333333326</v>
+        <v>3.8854166666666661</v>
       </c>
       <c r="G31" s="7">
         <f>H2-F31+H2</f>
-        <v>1.6145833333333344</v>
+        <v>1.5312500000000009</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1260,11 +1260,11 @@
       </c>
       <c r="F32" s="7">
         <f t="shared" si="1"/>
-        <v>3.8020833333333326</v>
+        <v>3.8854166666666661</v>
       </c>
       <c r="G32" s="7">
         <f>H2-F32+H2</f>
-        <v>1.6145833333333344</v>
+        <v>1.5312500000000009</v>
       </c>
     </row>
     <row r="33" spans="4:7" x14ac:dyDescent="0.25">
@@ -1274,11 +1274,11 @@
       </c>
       <c r="F33" s="7">
         <f t="shared" si="1"/>
-        <v>3.8020833333333326</v>
+        <v>3.8854166666666661</v>
       </c>
       <c r="G33" s="7">
         <f>H2-F33+H2</f>
-        <v>1.6145833333333344</v>
+        <v>1.5312500000000009</v>
       </c>
     </row>
     <row r="34" spans="4:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Bugfixes + Skill Increase + design features
Bugfixes:
- Random gen korjaus, ei enää system sleep, eli optimointia
- Initial feat stats
- stat boost duplicates
- class feat choices

Skill Increase:
- skillin noston valinnan rajoitin levelin suhteen

Design Choices:
- Mitä voidaan kovakoodata
- Mitkä pienet yksityiskohdat jäävät pois tästä versiosta, koska ei olisi kasvatettavissa järkevästi, eli täytyisi kuitenkin kokonaan luoda uudestaan, jos tulee esimerkiksi uusia jumalian peliin (usein tapahtuu)
- Mitä jätetään pelaajan selvitettäväksi, koska kyseessä on random gen, ei pysyvä character sheet. Osa asioista pelaajan täytyy selvittää itse esimerkiksi Focus Pool määrä.
- Medium Armor -- Warpriest/Ruffian?
</commit_message>
<xml_diff>
--- a/aikataulutus/Tyotunnit.xlsx
+++ b/aikataulutus/Tyotunnit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riku\Koulu\Ohjelmointyo\aikataulutus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2A6B5E-A9DD-4B75-A71B-2A3DF263640E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73874CBD-18D0-416B-8A55-45181B85E7FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2910" yWindow="1395" windowWidth="19665" windowHeight="12780" xr2:uid="{645D6CBF-11AA-407D-8E7D-16FD02D07F5D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Paivamaara</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>proficiencies + levelup (main stat weight) + BUGFIX + suunnittelua(1h?)</t>
+  </si>
+  <si>
+    <t>visual studio hajonnut - n. 3 tuntia korjaukseen</t>
+  </si>
+  <si>
+    <t>Bugfixes/Skill Increase/feature designs</t>
   </si>
 </sst>
 </file>
@@ -501,7 +507,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,11 +1174,16 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>44091</v>
+      </c>
       <c r="D26" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E26" s="8"/>
+      <c r="E26" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="F26" s="7">
         <f t="shared" si="1"/>
         <v>3.8854166666666661</v>
@@ -1183,18 +1194,29 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>44091</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.95833333333333337</v>
+      </c>
       <c r="D27" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E27" s="8"/>
+        <v>0.16666666666666674</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="F27" s="7">
         <f t="shared" si="1"/>
-        <v>3.8854166666666661</v>
+        <v>4.052083333333333</v>
       </c>
       <c r="G27" s="7">
         <f>H2-F27+H2</f>
-        <v>1.5312500000000009</v>
+        <v>1.3645833333333339</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1204,11 +1226,11 @@
       </c>
       <c r="F28" s="7">
         <f t="shared" si="1"/>
-        <v>3.8854166666666661</v>
+        <v>4.052083333333333</v>
       </c>
       <c r="G28" s="7">
         <f>H2-F28+H2</f>
-        <v>1.5312500000000009</v>
+        <v>1.3645833333333339</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1218,11 +1240,11 @@
       </c>
       <c r="F29" s="7">
         <f t="shared" si="1"/>
-        <v>3.8854166666666661</v>
+        <v>4.052083333333333</v>
       </c>
       <c r="G29" s="7">
         <f>H2-F29+H2</f>
-        <v>1.5312500000000009</v>
+        <v>1.3645833333333339</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1232,11 +1254,11 @@
       </c>
       <c r="F30" s="7">
         <f t="shared" si="1"/>
-        <v>3.8854166666666661</v>
+        <v>4.052083333333333</v>
       </c>
       <c r="G30" s="7">
         <f>H2-F30+H2</f>
-        <v>1.5312500000000009</v>
+        <v>1.3645833333333339</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1246,11 +1268,11 @@
       </c>
       <c r="F31" s="7">
         <f t="shared" si="1"/>
-        <v>3.8854166666666661</v>
+        <v>4.052083333333333</v>
       </c>
       <c r="G31" s="7">
         <f>H2-F31+H2</f>
-        <v>1.5312500000000009</v>
+        <v>1.3645833333333339</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1260,11 +1282,11 @@
       </c>
       <c r="F32" s="7">
         <f t="shared" si="1"/>
-        <v>3.8854166666666661</v>
+        <v>4.052083333333333</v>
       </c>
       <c r="G32" s="7">
         <f>H2-F32+H2</f>
-        <v>1.5312500000000009</v>
+        <v>1.3645833333333339</v>
       </c>
     </row>
     <row r="33" spans="4:7" x14ac:dyDescent="0.25">
@@ -1274,11 +1296,11 @@
       </c>
       <c r="F33" s="7">
         <f t="shared" si="1"/>
-        <v>3.8854166666666661</v>
+        <v>4.052083333333333</v>
       </c>
       <c r="G33" s="7">
         <f>H2-F33+H2</f>
-        <v>1.5312500000000009</v>
+        <v>1.3645833333333339</v>
       </c>
     </row>
     <row r="34" spans="4:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
4x Free boost + Initial Feat + UI
4x Free boost
- ratkaistiin hahmon luonnin 4x Free boost käsittely ja niiden omat vaatimukset ja rajoitteet

Initial Feat
- Ruffian ja Warpriest (rogue ja cleric) initial feat medium armor ongelma ratkaistu. Tosin ei siistein ratkaisu

UI:
- uudelleenrakennetaan UI:ta sopivammaksi ohjelman viimeistelyn näkökulmasta
</commit_message>
<xml_diff>
--- a/aikataulutus/Tyotunnit.xlsx
+++ b/aikataulutus/Tyotunnit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riku\Koulu\Ohjelmointyo\aikataulutus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73874CBD-18D0-416B-8A55-45181B85E7FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29F7CD2-8B51-4316-BA52-F3AF72AC456D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2910" yWindow="1395" windowWidth="19665" windowHeight="12780" xr2:uid="{645D6CBF-11AA-407D-8E7D-16FD02D07F5D}"/>
   </bookViews>
@@ -507,7 +507,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1220,17 +1220,26 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>44092</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.83333333333333337</v>
+      </c>
       <c r="D28" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="F28" s="7">
         <f t="shared" si="1"/>
-        <v>4.052083333333333</v>
+        <v>4.302083333333333</v>
       </c>
       <c r="G28" s="7">
         <f>H2-F28+H2</f>
-        <v>1.3645833333333339</v>
+        <v>1.1145833333333339</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1240,11 +1249,11 @@
       </c>
       <c r="F29" s="7">
         <f t="shared" si="1"/>
-        <v>4.052083333333333</v>
+        <v>4.302083333333333</v>
       </c>
       <c r="G29" s="7">
         <f>H2-F29+H2</f>
-        <v>1.3645833333333339</v>
+        <v>1.1145833333333339</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1254,11 +1263,11 @@
       </c>
       <c r="F30" s="7">
         <f t="shared" si="1"/>
-        <v>4.052083333333333</v>
+        <v>4.302083333333333</v>
       </c>
       <c r="G30" s="7">
         <f>H2-F30+H2</f>
-        <v>1.3645833333333339</v>
+        <v>1.1145833333333339</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1268,11 +1277,11 @@
       </c>
       <c r="F31" s="7">
         <f t="shared" si="1"/>
-        <v>4.052083333333333</v>
+        <v>4.302083333333333</v>
       </c>
       <c r="G31" s="7">
         <f>H2-F31+H2</f>
-        <v>1.3645833333333339</v>
+        <v>1.1145833333333339</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1282,11 +1291,11 @@
       </c>
       <c r="F32" s="7">
         <f t="shared" si="1"/>
-        <v>4.052083333333333</v>
+        <v>4.302083333333333</v>
       </c>
       <c r="G32" s="7">
         <f>H2-F32+H2</f>
-        <v>1.3645833333333339</v>
+        <v>1.1145833333333339</v>
       </c>
     </row>
     <row r="33" spans="4:7" x14ac:dyDescent="0.25">
@@ -1296,11 +1305,11 @@
       </c>
       <c r="F33" s="7">
         <f t="shared" si="1"/>
-        <v>4.052083333333333</v>
+        <v>4.302083333333333</v>
       </c>
       <c r="G33" s="7">
         <f>H2-F33+H2</f>
-        <v>1.3645833333333339</v>
+        <v>1.1145833333333339</v>
       </c>
     </row>
     <row r="34" spans="4:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Unity UI + XML + Scripts
Unity UI:
- kokonaan tabien redesign

XML:
- yhtäläisyyksien virheet joita tulee nyt esille paremmin UI:n kautta

Scripts:
- Unity UI rakentaminen, useita eri iteraatioita ja tämän pitäisi toimia parhaiten kaikille sivuille?
</commit_message>
<xml_diff>
--- a/aikataulutus/Tyotunnit.xlsx
+++ b/aikataulutus/Tyotunnit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riku\Koulu\Ohjelmointyo\aikataulutus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29F7CD2-8B51-4316-BA52-F3AF72AC456D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB09547-A7EF-4B38-8527-C205DDB4C6C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2910" yWindow="1395" windowWidth="19665" windowHeight="12780" xr2:uid="{645D6CBF-11AA-407D-8E7D-16FD02D07F5D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Paivamaara</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>Bugfixes/Skill Increase/feature designs</t>
+  </si>
+  <si>
+    <t>Unity UI redesign + XML + scripts + 4 Free Boost + Initial Feats</t>
   </si>
 </sst>
 </file>
@@ -507,7 +510,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1219,7 +1222,7 @@
         <v>1.3645833333333339</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44092</v>
       </c>
@@ -1227,19 +1230,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C28" s="2">
-        <v>0.83333333333333337</v>
+        <v>0.8125</v>
       </c>
       <c r="D28" s="6">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>0.22916666666666663</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="F28" s="7">
         <f t="shared" si="1"/>
-        <v>4.302083333333333</v>
+        <v>4.28125</v>
       </c>
       <c r="G28" s="7">
         <f>H2-F28+H2</f>
-        <v>1.1145833333333339</v>
+        <v>1.135416666666667</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1249,11 +1255,11 @@
       </c>
       <c r="F29" s="7">
         <f t="shared" si="1"/>
-        <v>4.302083333333333</v>
+        <v>4.28125</v>
       </c>
       <c r="G29" s="7">
         <f>H2-F29+H2</f>
-        <v>1.1145833333333339</v>
+        <v>1.135416666666667</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1263,11 +1269,11 @@
       </c>
       <c r="F30" s="7">
         <f t="shared" si="1"/>
-        <v>4.302083333333333</v>
+        <v>4.28125</v>
       </c>
       <c r="G30" s="7">
         <f>H2-F30+H2</f>
-        <v>1.1145833333333339</v>
+        <v>1.135416666666667</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1277,11 +1283,11 @@
       </c>
       <c r="F31" s="7">
         <f t="shared" si="1"/>
-        <v>4.302083333333333</v>
+        <v>4.28125</v>
       </c>
       <c r="G31" s="7">
         <f>H2-F31+H2</f>
-        <v>1.1145833333333339</v>
+        <v>1.135416666666667</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1291,11 +1297,11 @@
       </c>
       <c r="F32" s="7">
         <f t="shared" si="1"/>
-        <v>4.302083333333333</v>
+        <v>4.28125</v>
       </c>
       <c r="G32" s="7">
         <f>H2-F32+H2</f>
-        <v>1.1145833333333339</v>
+        <v>1.135416666666667</v>
       </c>
     </row>
     <row r="33" spans="4:7" x14ac:dyDescent="0.25">
@@ -1305,11 +1311,11 @@
       </c>
       <c r="F33" s="7">
         <f t="shared" si="1"/>
-        <v>4.302083333333333</v>
+        <v>4.28125</v>
       </c>
       <c r="G33" s="7">
         <f>H2-F33+H2</f>
-        <v>1.1145833333333339</v>
+        <v>1.135416666666667</v>
       </c>
     </row>
     <row r="34" spans="4:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Suunnitelmaa + Bugs + XML fix + Skills
Suunnitelmaa:
- Paivan_suunnitelma dokumentti
- Sisaltaa loydetyt Bugit

Bugs:
- refer Suunnitelmaa

XML fix:
- Dokumenttien läpikäyntiä, korjauksia.

Skills:
- Unity skills toimii, muutoksia myös alustukseen ja muiden sivujen toimintaan. Välilehtien aktiivisuuden suhteen ongelmia, maininta Suunnitelmassa.
</commit_message>
<xml_diff>
--- a/aikataulutus/Tyotunnit.xlsx
+++ b/aikataulutus/Tyotunnit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riku\Koulu\Ohjelmointyo\aikataulutus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC27603-ABA8-4DC9-818C-9BED8AC779FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7D9F99-CE6D-41F4-AA71-641FB16FB7A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34725" yWindow="2115" windowWidth="19665" windowHeight="12780" xr2:uid="{645D6CBF-11AA-407D-8E7D-16FD02D07F5D}"/>
   </bookViews>
@@ -510,7 +510,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,19 +1256,19 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="C29" s="2">
-        <v>0.89583333333333337</v>
+        <v>0.90625</v>
       </c>
       <c r="D29" s="6">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>0.26041666666666663</v>
       </c>
       <c r="F29" s="7">
         <f t="shared" si="1"/>
-        <v>4.53125</v>
+        <v>4.541666666666667</v>
       </c>
       <c r="G29" s="7">
         <f>H2-F29+H2</f>
-        <v>0.88541666666666696</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1278,11 +1278,11 @@
       </c>
       <c r="F30" s="7">
         <f t="shared" si="1"/>
-        <v>4.53125</v>
+        <v>4.541666666666667</v>
       </c>
       <c r="G30" s="7">
         <f>H2-F30+H2</f>
-        <v>0.88541666666666696</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1292,11 +1292,11 @@
       </c>
       <c r="F31" s="7">
         <f t="shared" si="1"/>
-        <v>4.53125</v>
+        <v>4.541666666666667</v>
       </c>
       <c r="G31" s="7">
         <f>H2-F31+H2</f>
-        <v>0.88541666666666696</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1306,11 +1306,11 @@
       </c>
       <c r="F32" s="7">
         <f t="shared" si="1"/>
-        <v>4.53125</v>
+        <v>4.541666666666667</v>
       </c>
       <c r="G32" s="7">
         <f>H2-F32+H2</f>
-        <v>0.88541666666666696</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="33" spans="4:7" x14ac:dyDescent="0.25">
@@ -1320,11 +1320,11 @@
       </c>
       <c r="F33" s="7">
         <f t="shared" si="1"/>
-        <v>4.53125</v>
+        <v>4.541666666666667</v>
       </c>
       <c r="G33" s="7">
         <f>H2-F33+H2</f>
-        <v>0.88541666666666696</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="34" spans="4:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Bugfixes + Pelin toimintaa
Bugfixes:
- Free boost duplicate kontrollointi
- 4 stat boost ajoitus
- Champion - class prerequisite
- Wizard Initial Feats
- Background identtiset valinnat kontrollointi
- Perception pois Skill Training kasvatuksesta
- Unity Tab activity toiminnallisuus useaa randomgenia varten

Pelin toimintaa:
- Skill Increase hahmon luonnissa lisätty
- Language Increase hahmon luonnissa korjattu (sekoitus Skill Increase kanssa)
- Initial Feats ominaisuuksia kovakoodattu, Tarvitsisi oman XML -tiedoston tämän osion kontrollointiin. Tehdään aliohjelma ongelman ohittamiseen. Tulevaisuudessa pitää lisätä XML (helpottaa mahdollisten uusien classien lisäämiseen)

TODO:
Wizard Arcane School ei toimi, tuottaa kaksi Arcane School lisaysta, Arcane School + Specialist tai Universalist, sijaan.
</commit_message>
<xml_diff>
--- a/aikataulutus/Tyotunnit.xlsx
+++ b/aikataulutus/Tyotunnit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riku\Koulu\Ohjelmointyo\aikataulutus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7D9F99-CE6D-41F4-AA71-641FB16FB7A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3EAC764-254C-4B53-A5F3-080DDE3307D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34725" yWindow="2115" windowWidth="19665" windowHeight="12780" xr2:uid="{645D6CBF-11AA-407D-8E7D-16FD02D07F5D}"/>
+    <workbookView xWindow="5220" yWindow="1140" windowWidth="19665" windowHeight="12780" xr2:uid="{645D6CBF-11AA-407D-8E7D-16FD02D07F5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -509,8 +509,8 @@
   <sheetPr codeName="Taul1"/>
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,17 +1272,26 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>44095</v>
+      </c>
+      <c r="B30" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.89583333333333337</v>
+      </c>
       <c r="D30" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="F30" s="7">
         <f t="shared" si="1"/>
-        <v>4.541666666666667</v>
+        <v>4.791666666666667</v>
       </c>
       <c r="G30" s="7">
         <f>H2-F30+H2</f>
-        <v>0.875</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1292,11 +1301,11 @@
       </c>
       <c r="F31" s="7">
         <f t="shared" si="1"/>
-        <v>4.541666666666667</v>
+        <v>4.791666666666667</v>
       </c>
       <c r="G31" s="7">
         <f>H2-F31+H2</f>
-        <v>0.875</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1306,11 +1315,11 @@
       </c>
       <c r="F32" s="7">
         <f t="shared" si="1"/>
-        <v>4.541666666666667</v>
+        <v>4.791666666666667</v>
       </c>
       <c r="G32" s="7">
         <f>H2-F32+H2</f>
-        <v>0.875</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="33" spans="4:7" x14ac:dyDescent="0.25">
@@ -1320,11 +1329,11 @@
       </c>
       <c r="F33" s="7">
         <f t="shared" si="1"/>
-        <v>4.541666666666667</v>
+        <v>4.791666666666667</v>
       </c>
       <c r="G33" s="7">
         <f>H2-F33+H2</f>
-        <v>0.875</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="34" spans="4:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Bugfixes + Frontpage UI design & Update + Randomgen
Bugfixes:
- Assurance feat ei lisatty.
- Background feat ei lisatty.
- Feat details ei lisatty.
- Lore increase bug (ensimmainen lore lisays ei kasvattanut) + koodin siistiminen.

Frontpage:
- kokonaan uusi redesign tärkeälle tiedolle.
- Frontpage Update rakennettu redesign aikana.

Randomgen:
- toimii inputin avulla ja pakottaa numerot 1-20 välille jos liian suuri (ilmenee kun generoi, peli antaa frontpage antaa levelin).
- Inputin kanssa meni paljon enemmän aikaa kuin oletin. Ongelmana oli TextMeshProUGUI:n kanssa tullu näkymätön elementti string muuttujaan, joka täytyi poistaa ennen kuin parse int muuttujaksi toimii. Jostakin syystä tämä ei ollut helposti löydettävissä netinkään avulla.
</commit_message>
<xml_diff>
--- a/aikataulutus/Tyotunnit.xlsx
+++ b/aikataulutus/Tyotunnit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riku\Koulu\Ohjelmointyo\aikataulutus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA771738-AC73-429A-846A-26501EEC48DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFF1D87-7529-4A8D-B4B1-E8C8DE7825A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5220" yWindow="1140" windowWidth="19665" windowHeight="12780" xr2:uid="{645D6CBF-11AA-407D-8E7D-16FD02D07F5D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Paivamaara</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>Unity UI redesign + XML + scripts + 4 Free Boost + Initial Feats</t>
+  </si>
+  <si>
+    <t>Bugfixes + Frontpage + Randomgen</t>
   </si>
 </sst>
 </file>
@@ -510,7 +513,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,17 +1298,29 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>44096</v>
+      </c>
+      <c r="B31" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.91666666666666663</v>
+      </c>
       <c r="D31" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.25</v>
+      </c>
+      <c r="E31" t="s">
+        <v>32</v>
       </c>
       <c r="F31" s="7">
         <f t="shared" si="1"/>
-        <v>4.84375</v>
+        <v>5.09375</v>
       </c>
       <c r="G31" s="7">
         <f>H2-F31+H2</f>
-        <v>0.57291666666666696</v>
+        <v>0.32291666666666696</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1315,11 +1330,11 @@
       </c>
       <c r="F32" s="7">
         <f t="shared" si="1"/>
-        <v>4.84375</v>
+        <v>5.09375</v>
       </c>
       <c r="G32" s="7">
         <f>H2-F32+H2</f>
-        <v>0.57291666666666696</v>
+        <v>0.32291666666666696</v>
       </c>
     </row>
     <row r="33" spans="4:7" x14ac:dyDescent="0.25">
@@ -1329,11 +1344,11 @@
       </c>
       <c r="F33" s="7">
         <f t="shared" si="1"/>
-        <v>4.84375</v>
+        <v>5.09375</v>
       </c>
       <c r="G33" s="7">
         <f>H2-F33+H2</f>
-        <v>0.57291666666666696</v>
+        <v>0.32291666666666696</v>
       </c>
     </row>
     <row r="34" spans="4:7" x14ac:dyDescent="0.25">

</xml_diff>